<commit_message>
modified initial values for piot points, ran pest to interpolate values to cells.
</commit_message>
<xml_diff>
--- a/Simulation_20160812T131753/EXCEL/SS_v_TR_wellIDs.xlsx
+++ b/Simulation_20160812T131753/EXCEL/SS_v_TR_wellIDs.xlsx
@@ -1512,9 +1512,6 @@
     <t>Druid Hills, in alluvium, impaced by pumping</t>
   </si>
   <si>
-    <t>gernal</t>
-  </si>
-  <si>
     <t>needs to be tighter</t>
   </si>
   <si>
@@ -1536,9 +1533,6 @@
     <t>Garlen Park, updstream of narrows, Cal-Am, impacted by high riparian GW ET</t>
   </si>
   <si>
-    <t>Near narrows, impaced by high GWET</t>
-  </si>
-  <si>
     <t>Scarlett</t>
   </si>
   <si>
@@ -1660,6 +1654,12 @@
   </si>
   <si>
     <t>Shelty Road, near 62</t>
+  </si>
+  <si>
+    <t>fit</t>
+  </si>
+  <si>
+    <t>Near narrows, impacted by high GWET</t>
   </si>
 </sst>
 </file>
@@ -1980,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H49" workbookViewId="0">
-      <selection activeCell="R65" sqref="R65"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2035,7 +2035,7 @@
         <v>357</v>
       </c>
       <c r="N1" t="s">
-        <v>495</v>
+        <v>543</v>
       </c>
       <c r="O1" t="s">
         <v>492</v>
@@ -2044,7 +2044,7 @@
         <v>421</v>
       </c>
       <c r="R1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
         <v>1.1883394355000001</v>
       </c>
       <c r="O2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P2" t="s">
         <v>358</v>
@@ -2170,10 +2170,10 @@
         <v>0.58668101292099994</v>
       </c>
       <c r="N4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P4" t="s">
         <v>360</v>
@@ -2220,10 +2220,10 @@
         <v>1.5633156608900001</v>
       </c>
       <c r="N5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P5" t="s">
         <v>361</v>
@@ -2270,10 +2270,10 @@
         <v>18.0432101817999</v>
       </c>
       <c r="N6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P6" t="s">
         <v>362</v>
@@ -2317,7 +2317,7 @@
         <v>2.0659332737199998</v>
       </c>
       <c r="O7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P7" t="s">
         <v>363</v>
@@ -2361,7 +2361,7 @@
         <v>3.8171819955599999</v>
       </c>
       <c r="O8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P8" t="s">
         <v>364</v>
@@ -2405,7 +2405,7 @@
         <v>0.413051034762</v>
       </c>
       <c r="O9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P9" t="s">
         <v>365</v>
@@ -2414,7 +2414,7 @@
         <v>101096</v>
       </c>
       <c r="R9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -2452,10 +2452,10 @@
         <v>3.92936153513</v>
       </c>
       <c r="N10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P10" t="s">
         <v>366</v>
@@ -2499,7 +2499,7 @@
         <v>3.7769565349600001</v>
       </c>
       <c r="O11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P11" t="s">
         <v>367</v>
@@ -2508,7 +2508,7 @@
         <v>101290</v>
       </c>
       <c r="R11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -2546,10 +2546,10 @@
         <v>3.3206180455099998</v>
       </c>
       <c r="N12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P12" t="s">
         <v>368</v>
@@ -2558,7 +2558,7 @@
         <v>101291</v>
       </c>
       <c r="R12" t="s">
-        <v>503</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -2596,10 +2596,10 @@
         <v>1.09747689211</v>
       </c>
       <c r="N13" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P13" t="s">
         <v>369</v>
@@ -2608,7 +2608,7 @@
         <v>101293</v>
       </c>
       <c r="R13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -2646,10 +2646,10 @@
         <v>2.3957454680599999</v>
       </c>
       <c r="N14" t="s">
+        <v>496</v>
+      </c>
+      <c r="O14" t="s">
         <v>497</v>
-      </c>
-      <c r="O14" t="s">
-        <v>498</v>
       </c>
       <c r="P14" t="s">
         <v>370</v>
@@ -2658,7 +2658,7 @@
         <v>101299</v>
       </c>
       <c r="R14" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -2696,7 +2696,7 @@
         <v>1.26373475737</v>
       </c>
       <c r="O15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P15" t="s">
         <v>371</v>
@@ -2705,7 +2705,7 @@
         <v>101300</v>
       </c>
       <c r="R15" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -2743,7 +2743,7 @@
         <v>3.3004646326399998</v>
       </c>
       <c r="O16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P16" t="s">
         <v>372</v>
@@ -2752,7 +2752,7 @@
         <v>101302</v>
       </c>
       <c r="R16" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -2790,7 +2790,7 @@
         <v>4.5504490678199998</v>
       </c>
       <c r="O17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P17" t="s">
         <v>373</v>
@@ -2799,7 +2799,7 @@
         <v>101303</v>
       </c>
       <c r="R17" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -2837,7 +2837,7 @@
         <v>2.2784390752100001</v>
       </c>
       <c r="O18" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P18" t="s">
         <v>374</v>
@@ -2846,7 +2846,7 @@
         <v>101305</v>
       </c>
       <c r="R18" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
@@ -2884,7 +2884,7 @@
         <v>1.2933808604199999</v>
       </c>
       <c r="O19" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P19" t="s">
         <v>375</v>
@@ -2893,7 +2893,7 @@
         <v>101317</v>
       </c>
       <c r="R19" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -2931,7 +2931,7 @@
         <v>1.3363772706199999</v>
       </c>
       <c r="O20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P20" t="s">
         <v>376</v>
@@ -2940,7 +2940,7 @@
         <v>101318</v>
       </c>
       <c r="R20" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -2978,7 +2978,7 @@
         <v>0.790012115332</v>
       </c>
       <c r="O21" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P21" t="s">
         <v>377</v>
@@ -2987,7 +2987,7 @@
         <v>101319</v>
       </c>
       <c r="R21" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -3025,7 +3025,7 @@
         <v>4.6417756577800002</v>
       </c>
       <c r="O22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P22" t="s">
         <v>378</v>
@@ -3034,7 +3034,7 @@
         <v>101320</v>
       </c>
       <c r="R22" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -3072,7 +3072,7 @@
         <v>2.6339186860099999</v>
       </c>
       <c r="O23" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P23" t="s">
         <v>379</v>
@@ -3081,7 +3081,7 @@
         <v>102028</v>
       </c>
       <c r="R23" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -3119,7 +3119,7 @@
         <v>3.4992669200900002</v>
       </c>
       <c r="O24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P24" t="s">
         <v>380</v>
@@ -3128,7 +3128,7 @@
         <v>102029</v>
       </c>
       <c r="R24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -3166,7 +3166,7 @@
         <v>2.7658079512499998</v>
       </c>
       <c r="O25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P25" t="s">
         <v>381</v>
@@ -3175,7 +3175,7 @@
         <v>102051</v>
       </c>
       <c r="R25" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -3213,7 +3213,7 @@
         <v>2.23049408297</v>
       </c>
       <c r="O26" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P26" t="s">
         <v>382</v>
@@ -3222,7 +3222,7 @@
         <v>102077</v>
       </c>
       <c r="R26" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
@@ -3260,7 +3260,7 @@
         <v>1.06315151545</v>
       </c>
       <c r="O27" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P27" t="s">
         <v>383</v>
@@ -3269,7 +3269,7 @@
         <v>102078</v>
       </c>
       <c r="R27" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -3307,7 +3307,7 @@
         <v>4.4037153015700001</v>
       </c>
       <c r="O28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P28" t="s">
         <v>384</v>
@@ -3316,7 +3316,7 @@
         <v>102079</v>
       </c>
       <c r="R28" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -3354,7 +3354,7 @@
         <v>2.6533131777199999</v>
       </c>
       <c r="O29" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P29" t="s">
         <v>385</v>
@@ -3363,7 +3363,7 @@
         <v>102080</v>
       </c>
       <c r="R29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -3401,7 +3401,7 @@
         <v>2.9575165356399999</v>
       </c>
       <c r="O30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P30" t="s">
         <v>386</v>
@@ -3410,7 +3410,7 @@
         <v>102083</v>
       </c>
       <c r="R30" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -3448,7 +3448,7 @@
         <v>2.4973625338300001</v>
       </c>
       <c r="O31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P31" t="s">
         <v>387</v>
@@ -3457,7 +3457,7 @@
         <v>102084</v>
       </c>
       <c r="R31" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -3495,7 +3495,7 @@
         <v>1.7034729553000001</v>
       </c>
       <c r="O32" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P32" t="s">
         <v>388</v>
@@ -3504,7 +3504,7 @@
         <v>102086</v>
       </c>
       <c r="R32" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
@@ -3542,10 +3542,10 @@
         <v>5.0001084199200001</v>
       </c>
       <c r="N33" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O33" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P33" t="s">
         <v>389</v>
@@ -3554,7 +3554,7 @@
         <v>102087</v>
       </c>
       <c r="R33" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
@@ -3592,10 +3592,10 @@
         <v>1.0837537718099999E-4</v>
       </c>
       <c r="N34" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O34" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P34" t="s">
         <v>390</v>
@@ -3604,7 +3604,7 @@
         <v>102093</v>
       </c>
       <c r="R34" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
@@ -3642,7 +3642,7 @@
         <v>2.54036544016</v>
       </c>
       <c r="O35" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P35" t="s">
         <v>391</v>
@@ -3651,7 +3651,7 @@
         <v>102094</v>
       </c>
       <c r="R35" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
@@ -3689,7 +3689,7 @@
         <v>4.6032567556900004</v>
       </c>
       <c r="O36" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P36" t="s">
         <v>392</v>
@@ -3698,7 +3698,7 @@
         <v>102096</v>
       </c>
       <c r="R36" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -3736,7 +3736,7 @@
         <v>4.01369747699</v>
       </c>
       <c r="O37" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P37" t="s">
         <v>393</v>
@@ -3745,7 +3745,7 @@
         <v>102097</v>
       </c>
       <c r="R37" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -3783,10 +3783,10 @@
         <v>1.4024796982900001</v>
       </c>
       <c r="N38" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O38" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P38" t="s">
         <v>394</v>
@@ -3795,7 +3795,7 @@
         <v>102100</v>
       </c>
       <c r="R38" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
@@ -3833,7 +3833,7 @@
         <v>4.7386614582400002</v>
       </c>
       <c r="O39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P39" t="s">
         <v>395</v>
@@ -3842,7 +3842,7 @@
         <v>102103</v>
       </c>
       <c r="R39" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
@@ -3880,7 +3880,7 @@
         <v>2.7732246087600001</v>
       </c>
       <c r="O40" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P40" t="s">
         <v>396</v>
@@ -3889,7 +3889,7 @@
         <v>102106</v>
       </c>
       <c r="R40" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
@@ -3927,7 +3927,7 @@
         <v>2.8769384254400001</v>
       </c>
       <c r="O41" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P41" t="s">
         <v>397</v>
@@ -3971,7 +3971,7 @@
         <v>4.0009039024300002</v>
       </c>
       <c r="O42" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P42" t="s">
         <v>398</v>
@@ -3980,7 +3980,7 @@
         <v>102110</v>
       </c>
       <c r="R42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -4018,7 +4018,7 @@
         <v>1.36122629143</v>
       </c>
       <c r="O43" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P43" t="s">
         <v>399</v>
@@ -4027,7 +4027,7 @@
         <v>102111</v>
       </c>
       <c r="R43" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -4065,10 +4065,10 @@
         <v>3.8571322349699999</v>
       </c>
       <c r="N44" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="O44" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P44" t="s">
         <v>400</v>
@@ -4077,7 +4077,7 @@
         <v>102112</v>
       </c>
       <c r="R44" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -4115,7 +4115,7 @@
         <v>1.9998915880000001</v>
       </c>
       <c r="O45" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P45" t="s">
         <v>401</v>
@@ -4124,7 +4124,7 @@
         <v>102113</v>
       </c>
       <c r="R45" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
@@ -4162,7 +4162,7 @@
         <v>0.497890190412</v>
       </c>
       <c r="O46" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P46" t="s">
         <v>402</v>
@@ -4171,7 +4171,7 @@
         <v>102170</v>
       </c>
       <c r="R46" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
@@ -4209,7 +4209,7 @@
         <v>0.74452624295299996</v>
       </c>
       <c r="O47" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P47" t="s">
         <v>403</v>
@@ -4218,7 +4218,7 @@
         <v>102177</v>
       </c>
       <c r="R47" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -4256,7 +4256,7 @@
         <v>1.4513825680600001</v>
       </c>
       <c r="O48" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P48" t="s">
         <v>404</v>
@@ -4265,7 +4265,7 @@
         <v>102179</v>
       </c>
       <c r="R48" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
@@ -4303,7 +4303,7 @@
         <v>0.16483880986499999</v>
       </c>
       <c r="O49" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P49" t="s">
         <v>405</v>
@@ -4312,7 +4312,7 @@
         <v>102197</v>
       </c>
       <c r="R49" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
@@ -4350,7 +4350,7 @@
         <v>3.9998915800799999</v>
       </c>
       <c r="O50" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P50" t="s">
         <v>406</v>
@@ -4359,7 +4359,7 @@
         <v>102272</v>
       </c>
       <c r="R50" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
@@ -4397,7 +4397,7 @@
         <v>2.7635761084000001</v>
       </c>
       <c r="O51" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P51" t="s">
         <v>407</v>
@@ -4406,7 +4406,7 @@
         <v>102312</v>
       </c>
       <c r="R51" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
@@ -4444,7 +4444,7 @@
         <v>2.0001084534500002</v>
       </c>
       <c r="O52" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P52" t="s">
         <v>408</v>
@@ -4453,7 +4453,7 @@
         <v>102393</v>
       </c>
       <c r="R52" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
@@ -4491,7 +4491,7 @@
         <v>0.469492695505</v>
       </c>
       <c r="O53" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P53" t="s">
         <v>409</v>
@@ -4500,7 +4500,7 @@
         <v>102396</v>
       </c>
       <c r="R53" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
@@ -4538,7 +4538,7 @@
         <v>1.0418920304499999</v>
       </c>
       <c r="O54" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P54" t="s">
         <v>410</v>
@@ -4547,7 +4547,7 @@
         <v>102397</v>
       </c>
       <c r="R54" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
@@ -4585,7 +4585,7 @@
         <v>3.7007248959700001</v>
       </c>
       <c r="O55" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P55" t="s">
         <v>411</v>
@@ -4594,7 +4594,7 @@
         <v>102427</v>
       </c>
       <c r="R55" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
@@ -4632,7 +4632,7 @@
         <v>1.7406443378599999E-2</v>
       </c>
       <c r="O56" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P56" t="s">
         <v>412</v>
@@ -4641,7 +4641,7 @@
         <v>102434</v>
       </c>
       <c r="R56" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
@@ -4679,7 +4679,7 @@
         <v>0.99989162845599999</v>
       </c>
       <c r="O57" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P57" t="s">
         <v>413</v>
@@ -4688,7 +4688,7 @@
         <v>102436</v>
       </c>
       <c r="R57" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
@@ -4726,7 +4726,7 @@
         <v>1.21996227919</v>
       </c>
       <c r="O58" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P58" t="s">
         <v>414</v>
@@ -4735,7 +4735,7 @@
         <v>102437</v>
       </c>
       <c r="R58" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
@@ -4773,7 +4773,7 @@
         <v>2.3490637486599999</v>
       </c>
       <c r="O59" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P59" t="s">
         <v>415</v>
@@ -4782,7 +4782,7 @@
         <v>102438</v>
       </c>
       <c r="R59" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
@@ -4820,7 +4820,7 @@
         <v>1.0001085079300001</v>
       </c>
       <c r="O60" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P60" t="s">
         <v>416</v>
@@ -4829,7 +4829,7 @@
         <v>102439</v>
       </c>
       <c r="R60" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
@@ -4867,7 +4867,7 @@
         <v>1.5638058481999999</v>
       </c>
       <c r="O61" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P61" t="s">
         <v>417</v>
@@ -4876,7 +4876,7 @@
         <v>102443</v>
       </c>
       <c r="R61" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
@@ -4914,7 +4914,7 @@
         <v>3.0459200667899999</v>
       </c>
       <c r="O62" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P62" t="s">
         <v>418</v>
@@ -4923,7 +4923,7 @@
         <v>102444</v>
       </c>
       <c r="R62" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
@@ -4961,7 +4961,7 @@
         <v>4.9514854159299997</v>
       </c>
       <c r="O63" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P63" t="s">
         <v>419</v>
@@ -4970,7 +4970,7 @@
         <v>102484</v>
       </c>
       <c r="R63" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
@@ -5008,7 +5008,7 @@
         <v>0.324576281977</v>
       </c>
       <c r="O64" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P64" t="s">
         <v>420</v>
@@ -5017,7 +5017,7 @@
         <v>102507</v>
       </c>
       <c r="R64" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>